<commit_message>
Resolving Municipalities on progress
</commit_message>
<xml_diff>
--- a/desinventar/LocalBody_VDC_MUNICIPALITY_for_drr_EDITED.xlsx
+++ b/desinventar/LocalBody_VDC_MUNICIPALITY_for_drr_EDITED.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\learn2code\desinventar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\learn2code\python_pandas\desinventar\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8025" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8025" tabRatio="322" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DRR_2_DES" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4892" uniqueCount="1741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4900" uniqueCount="1744">
   <si>
     <t>District</t>
   </si>
@@ -5249,6 +5249,15 @@
   </si>
   <si>
     <t>Jit Bdr. Thapa</t>
+  </si>
+  <si>
+    <t>Lete</t>
+  </si>
+  <si>
+    <t>Pandav Gupha</t>
+  </si>
+  <si>
+    <t>Tribeni Nalagad</t>
   </si>
 </sst>
 </file>
@@ -19913,132 +19922,130 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB20"/>
+  <dimension ref="A1:AD20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB22" sqref="AB22"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
         <v>1682</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1683</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>1684</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>1685</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>1686</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>1687</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>1688</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>1689</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>1690</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>1691</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>1692</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>1693</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>1694</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>1695</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>1696</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>1697</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>1698</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>1699</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>1700</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>1701</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>1702</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>1703</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>1704</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>1705</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>1706</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>1707</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C2">
         <v>11759</v>
       </c>
-      <c r="B2">
+      <c r="D2">
         <v>32</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>82</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>83</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>6</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>43105</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>1708</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -20050,16 +20057,16 @@
         <v>0</v>
       </c>
       <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
         <v>1</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>300000</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -20086,42 +20093,42 @@
         <v>0</v>
       </c>
       <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
         <v>1</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>1709</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AD2" t="s">
         <v>1710</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C3">
         <v>11810</v>
       </c>
-      <c r="B3">
+      <c r="D3">
         <v>83</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>163</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>1711</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>43109</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>1708</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -20133,16 +20140,16 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
       </c>
       <c r="P3">
         <v>1</v>
       </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
       <c r="R3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3">
         <v>0</v>
@@ -20168,40 +20175,40 @@
       <c r="Z3">
         <v>0</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="s">
         <v>1709</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AD3" t="s">
         <v>1712</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C4">
         <v>11820</v>
       </c>
-      <c r="B4">
+      <c r="D4">
         <v>93</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>63</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>177</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>6</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>43109</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>1708</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -20213,28 +20220,28 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4">
-        <v>55000</v>
+        <v>0</v>
       </c>
       <c r="P4">
         <v>1</v>
       </c>
       <c r="Q4">
+        <v>55000</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
         <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>1</v>
       </c>
       <c r="T4">
         <v>0</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V4">
         <v>0</v>
@@ -20251,40 +20258,40 @@
       <c r="Z4">
         <v>0</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="s">
         <v>1709</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AD4" t="s">
         <v>1713</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C5">
         <v>11895</v>
       </c>
-      <c r="B5">
+      <c r="D5">
         <v>168</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>56</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>282</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>3</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>43113</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>1708</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -20296,16 +20303,16 @@
         <v>0</v>
       </c>
       <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
         <v>1</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>200000</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -20329,45 +20336,45 @@
         <v>0</v>
       </c>
       <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
         <v>2</v>
       </c>
-      <c r="Z5">
+      <c r="AB5">
         <v>1</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AC5" t="s">
         <v>1709</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AD5" t="s">
         <v>1714</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C6">
         <v>11902</v>
       </c>
-      <c r="B6">
+      <c r="D6">
         <v>175</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>82</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>286</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>6</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>43113</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>1708</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -20379,28 +20386,28 @@
         <v>0</v>
       </c>
       <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
         <v>1</v>
       </c>
-      <c r="O6">
+      <c r="Q6">
         <v>365000</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
       </c>
       <c r="R6">
         <v>0</v>
       </c>
       <c r="S6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T6">
         <v>0</v>
       </c>
       <c r="U6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6">
         <v>0</v>
@@ -20417,40 +20424,40 @@
       <c r="Z6">
         <v>0</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="s">
         <v>1709</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AD6" t="s">
         <v>1715</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C7">
         <v>11912</v>
       </c>
-      <c r="B7">
+      <c r="D7">
         <v>185</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>294</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>295</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>1</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>43115</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>1708</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -20462,28 +20469,28 @@
         <v>0</v>
       </c>
       <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
         <v>1</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
         <v>300000</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
       </c>
       <c r="R7">
         <v>0</v>
       </c>
       <c r="S7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T7">
         <v>0</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7">
         <v>0</v>
@@ -20500,40 +20507,40 @@
       <c r="Z7">
         <v>0</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7" t="s">
         <v>1709</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AD7" t="s">
         <v>1716</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C8">
         <v>12006</v>
       </c>
-      <c r="B8">
+      <c r="D8">
         <v>279</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>294</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>404</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>1</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>43127</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>1708</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -20545,25 +20552,25 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
       </c>
       <c r="P8">
         <v>1</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
         <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>7</v>
       </c>
       <c r="T8">
         <v>0</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="V8">
         <v>0</v>
@@ -20575,45 +20582,45 @@
         <v>0</v>
       </c>
       <c r="Y8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Z8">
         <v>0</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AA8">
+        <v>4</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8" t="s">
         <v>1709</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AD8" t="s">
         <v>1717</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C9">
         <v>12021</v>
       </c>
-      <c r="B9">
+      <c r="D9">
         <v>294</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>294</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>418</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>6</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>43130</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>1708</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -20625,28 +20632,28 @@
         <v>0</v>
       </c>
       <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
         <v>1</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>500000</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
       </c>
       <c r="R9">
         <v>0</v>
       </c>
       <c r="S9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T9">
         <v>0</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V9">
         <v>0</v>
@@ -20663,40 +20670,40 @@
       <c r="Z9">
         <v>0</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9" t="s">
         <v>1718</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AD9" t="s">
         <v>1719</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C10">
         <v>12210</v>
       </c>
-      <c r="B10">
+      <c r="D10">
         <v>483</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>32</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>621</v>
       </c>
-      <c r="E10">
+      <c r="G10">
         <v>3</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>43152</v>
       </c>
-      <c r="H10" t="s">
+      <c r="J10" t="s">
         <v>1708</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -20708,28 +20715,28 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O10">
-        <v>1256000</v>
+        <v>0</v>
       </c>
       <c r="P10">
         <v>1</v>
       </c>
       <c r="Q10">
+        <v>1256000</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
         <v>0</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>1</v>
       </c>
       <c r="T10">
         <v>0</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10">
         <v>0</v>
@@ -20746,40 +20753,40 @@
       <c r="Z10">
         <v>0</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10" t="s">
         <v>1709</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AD10" t="s">
         <v>1720</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C11">
         <v>12261</v>
       </c>
-      <c r="B11">
+      <c r="D11">
         <v>534</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>166</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>652</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11" t="s">
         <v>1721</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>43159</v>
       </c>
-      <c r="H11" t="s">
+      <c r="J11" t="s">
         <v>1708</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -20791,28 +20798,28 @@
         <v>0</v>
       </c>
       <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
         <v>1</v>
       </c>
-      <c r="O11">
+      <c r="Q11">
         <v>60000</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
       </c>
       <c r="R11">
         <v>0</v>
       </c>
       <c r="S11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T11">
         <v>0</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V11">
         <v>0</v>
@@ -20829,61 +20836,61 @@
       <c r="Z11">
         <v>0</v>
       </c>
-      <c r="AA11" t="s">
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11" t="s">
         <v>1709</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AD11" t="s">
         <v>1722</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C12">
         <v>13383</v>
       </c>
-      <c r="B12">
+      <c r="D12">
         <v>1656</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>179</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>1114</v>
       </c>
-      <c r="E12">
+      <c r="G12">
         <v>2</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>43251</v>
       </c>
-      <c r="H12" t="s">
+      <c r="J12" t="s">
         <v>1723</v>
       </c>
-      <c r="I12">
+      <c r="K12">
         <v>2</v>
       </c>
-      <c r="J12">
+      <c r="L12">
         <v>1</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>3</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
       <c r="N12">
+        <v>3</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
         <v>2</v>
       </c>
-      <c r="P12">
+      <c r="R12">
         <v>1</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="R12">
-        <v>0</v>
       </c>
       <c r="S12">
         <v>0</v>
@@ -20909,40 +20916,40 @@
       <c r="Z12">
         <v>0</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12" t="s">
         <v>1709</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AD12" t="s">
         <v>1724</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C13">
         <v>13471</v>
       </c>
-      <c r="B13">
+      <c r="D13">
         <v>1744</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>473</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" t="s">
         <v>1139</v>
       </c>
-      <c r="E13">
+      <c r="G13">
         <v>5</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <v>43260</v>
       </c>
-      <c r="H13" t="s">
+      <c r="J13" t="s">
         <v>1725</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -20954,16 +20961,16 @@
         <v>0</v>
       </c>
       <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
         <v>1</v>
       </c>
-      <c r="O13">
+      <c r="Q13">
         <v>15000000</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
       </c>
       <c r="R13">
         <v>0</v>
@@ -20992,40 +20999,40 @@
       <c r="Z13">
         <v>0</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13" t="s">
         <v>1709</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AD13" t="s">
         <v>1726</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C14">
         <v>13999</v>
       </c>
-      <c r="B14">
+      <c r="D14">
         <v>2272</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
         <v>463</v>
       </c>
-      <c r="D14" t="s">
+      <c r="F14" t="s">
         <v>1252</v>
       </c>
-      <c r="E14">
+      <c r="G14">
         <v>14</v>
       </c>
-      <c r="G14">
+      <c r="I14">
         <v>43316</v>
       </c>
-      <c r="H14" t="s">
+      <c r="J14" t="s">
         <v>1727</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -21037,16 +21044,16 @@
         <v>0</v>
       </c>
       <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
         <v>1</v>
       </c>
-      <c r="O14">
+      <c r="Q14">
         <v>60000</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <v>0</v>
       </c>
       <c r="R14">
         <v>0</v>
@@ -21055,13 +21062,13 @@
         <v>0</v>
       </c>
       <c r="T14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U14">
         <v>0</v>
       </c>
       <c r="V14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W14">
         <v>0</v>
@@ -21075,40 +21082,46 @@
       <c r="Z14">
         <v>0</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14" t="s">
         <v>1728</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="AD14" t="s">
         <v>1729</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1743</v>
+      </c>
+      <c r="C15">
         <v>14137</v>
       </c>
-      <c r="B15">
+      <c r="D15">
         <v>2410</v>
       </c>
-      <c r="C15" t="s">
+      <c r="E15" t="s">
         <v>35</v>
       </c>
-      <c r="D15" t="s">
+      <c r="F15" t="s">
         <v>1277</v>
       </c>
-      <c r="E15">
+      <c r="G15">
         <v>12</v>
       </c>
-      <c r="G15">
+      <c r="I15">
         <v>43326</v>
       </c>
-      <c r="H15" t="s">
+      <c r="J15" t="s">
         <v>1727</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -21120,28 +21133,28 @@
         <v>0</v>
       </c>
       <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
         <v>2</v>
       </c>
-      <c r="O15">
+      <c r="Q15">
         <v>1058000</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
       </c>
       <c r="R15">
         <v>0</v>
       </c>
       <c r="S15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T15">
         <v>0</v>
       </c>
       <c r="U15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V15">
         <v>0</v>
@@ -21158,40 +21171,46 @@
       <c r="Z15">
         <v>0</v>
       </c>
-      <c r="AA15" t="s">
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15" t="s">
         <v>1730</v>
       </c>
-      <c r="AB15" t="s">
+      <c r="AD15" t="s">
         <v>1731</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1742</v>
+      </c>
+      <c r="C16">
         <v>14419</v>
       </c>
-      <c r="B16">
+      <c r="D16">
         <v>2692</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>363</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16" t="s">
         <v>1320</v>
       </c>
-      <c r="E16">
+      <c r="G16">
         <v>5</v>
       </c>
-      <c r="G16">
+      <c r="I16">
         <v>43349</v>
       </c>
-      <c r="H16" t="s">
+      <c r="J16" t="s">
         <v>1723</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -21203,13 +21222,13 @@
         <v>0</v>
       </c>
       <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
         <v>2</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
       </c>
       <c r="R16">
         <v>0</v>
@@ -21233,48 +21252,54 @@
         <v>0</v>
       </c>
       <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16">
         <v>6</v>
       </c>
-      <c r="Z16">
+      <c r="AB16">
         <v>2</v>
       </c>
-      <c r="AA16" t="s">
+      <c r="AC16" t="s">
         <v>1732</v>
       </c>
-      <c r="AB16" t="s">
+      <c r="AD16" t="s">
         <v>1733</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1741</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C17">
         <v>14647</v>
       </c>
-      <c r="B17">
+      <c r="D17">
         <v>2920</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
         <v>242</v>
       </c>
-      <c r="D17" t="s">
+      <c r="F17" t="s">
         <v>1345</v>
       </c>
-      <c r="G17">
+      <c r="I17">
         <v>43375</v>
       </c>
-      <c r="H17" t="s">
+      <c r="J17" t="s">
         <v>1734</v>
       </c>
-      <c r="I17">
+      <c r="K17">
         <v>1</v>
       </c>
-      <c r="J17">
+      <c r="L17">
         <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>1</v>
       </c>
       <c r="M17">
         <v>0</v>
@@ -21282,11 +21307,11 @@
       <c r="N17">
         <v>1</v>
       </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
       <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17">
         <v>0</v>
@@ -21315,40 +21340,40 @@
       <c r="Z17">
         <v>0</v>
       </c>
-      <c r="AA17" t="s">
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17" t="s">
         <v>1709</v>
       </c>
-      <c r="AB17" t="s">
+      <c r="AD17" t="s">
         <v>1735</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C18">
         <v>15278</v>
       </c>
-      <c r="B18">
+      <c r="D18">
         <v>3551</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
         <v>363</v>
       </c>
-      <c r="D18" t="s">
+      <c r="F18" t="s">
         <v>1382</v>
       </c>
-      <c r="E18">
+      <c r="G18">
         <v>4</v>
       </c>
-      <c r="G18">
+      <c r="I18">
         <v>43438</v>
       </c>
-      <c r="H18" t="s">
+      <c r="J18" t="s">
         <v>1736</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -21360,16 +21385,16 @@
         <v>0</v>
       </c>
       <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
         <v>1</v>
       </c>
-      <c r="P18">
+      <c r="R18">
         <v>2</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <v>0</v>
       </c>
       <c r="S18">
         <v>0</v>
@@ -21395,37 +21420,37 @@
       <c r="Z18">
         <v>0</v>
       </c>
-      <c r="AB18" t="s">
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AD18" t="s">
         <v>1737</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C19">
         <v>17706</v>
       </c>
-      <c r="B19">
+      <c r="D19">
         <v>5979</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E19" t="s">
         <v>242</v>
       </c>
-      <c r="D19" t="s">
+      <c r="F19" t="s">
         <v>1468</v>
       </c>
-      <c r="E19">
+      <c r="G19">
         <v>3</v>
       </c>
-      <c r="G19">
+      <c r="I19">
         <v>43608</v>
       </c>
-      <c r="H19" t="s">
+      <c r="J19" t="s">
         <v>1708</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -21437,28 +21462,28 @@
         <v>0</v>
       </c>
       <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
         <v>1</v>
       </c>
-      <c r="O19">
+      <c r="Q19">
         <v>295000</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
       </c>
       <c r="R19">
         <v>0</v>
       </c>
       <c r="S19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T19">
         <v>0</v>
       </c>
       <c r="U19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V19">
         <v>0</v>
@@ -21475,43 +21500,49 @@
       <c r="Z19">
         <v>0</v>
       </c>
-      <c r="AA19" t="s">
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AB19">
+        <v>0</v>
+      </c>
+      <c r="AC19" t="s">
         <v>1709</v>
       </c>
-      <c r="AB19" t="s">
+      <c r="AD19" t="s">
         <v>1738</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1510</v>
+      </c>
+      <c r="B20" t="s">
+        <v>567</v>
+      </c>
+      <c r="C20">
         <v>20208</v>
       </c>
-      <c r="B20">
+      <c r="D20">
         <v>8481</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>153</v>
       </c>
-      <c r="D20" t="s">
+      <c r="F20" t="s">
         <v>1510</v>
       </c>
-      <c r="E20">
+      <c r="G20">
         <v>5</v>
       </c>
-      <c r="F20" t="s">
+      <c r="H20" t="s">
         <v>1739</v>
       </c>
-      <c r="G20">
+      <c r="I20">
         <v>43832</v>
       </c>
-      <c r="H20" t="s">
+      <c r="J20" t="s">
         <v>1708</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -21523,28 +21554,28 @@
         <v>0</v>
       </c>
       <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
         <v>1</v>
       </c>
-      <c r="O20">
+      <c r="Q20">
         <v>1017500</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
       </c>
       <c r="R20">
         <v>0</v>
       </c>
       <c r="S20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T20">
         <v>0</v>
       </c>
       <c r="U20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V20">
         <v>0</v>
@@ -21559,9 +21590,15 @@
         <v>0</v>
       </c>
       <c r="Z20">
+        <v>0</v>
+      </c>
+      <c r="AA20">
+        <v>0</v>
+      </c>
+      <c r="AB20">
         <v>1</v>
       </c>
-      <c r="AB20" t="s">
+      <c r="AD20" t="s">
         <v>1740</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Creating matching list of District and VDC - on progress
</commit_message>
<xml_diff>
--- a/desinventar/LocalBody_VDC_MUNICIPALITY_for_drr_EDITED.xlsx
+++ b/desinventar/LocalBody_VDC_MUNICIPALITY_for_drr_EDITED.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8025" tabRatio="322"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8025" tabRatio="624" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="DRR_2_DES" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4910" uniqueCount="1753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4926" uniqueCount="1753">
   <si>
     <t>District</t>
   </si>
@@ -6114,7 +6114,7 @@
   </sheetPr>
   <dimension ref="A1:E815"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D395" sqref="D395"/>
     </sheetView>
   </sheetViews>
@@ -19981,7 +19981,7 @@
   <dimension ref="A1:AC20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24825,16 +24825,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E220"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="D220" sqref="D220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -24881,6 +24881,9 @@
       <c r="C3" t="s">
         <v>1252</v>
       </c>
+      <c r="D3" t="s">
+        <v>465</v>
+      </c>
       <c r="E3" t="s">
         <v>1252</v>
       </c>
@@ -25116,6 +25119,9 @@
       <c r="C17" t="s">
         <v>1320</v>
       </c>
+      <c r="D17" t="s">
+        <v>1741</v>
+      </c>
       <c r="E17" t="s">
         <v>1321</v>
       </c>
@@ -25130,6 +25136,9 @@
       <c r="C18" t="s">
         <v>1382</v>
       </c>
+      <c r="D18" t="s">
+        <v>1751</v>
+      </c>
       <c r="E18" t="s">
         <v>1383</v>
       </c>
@@ -26266,6 +26275,9 @@
       <c r="C85" t="s">
         <v>1277</v>
       </c>
+      <c r="D85" t="s">
+        <v>1742</v>
+      </c>
       <c r="E85" t="s">
         <v>1278</v>
       </c>
@@ -26705,6 +26717,9 @@
       <c r="C111" t="s">
         <v>621</v>
       </c>
+      <c r="D111" t="s">
+        <v>1744</v>
+      </c>
       <c r="E111" t="s">
         <v>622</v>
       </c>
@@ -26804,6 +26819,9 @@
       <c r="C117" t="s">
         <v>652</v>
       </c>
+      <c r="D117" t="s">
+        <v>1604</v>
+      </c>
       <c r="E117" t="s">
         <v>652</v>
       </c>
@@ -27472,6 +27490,9 @@
       <c r="C157" t="s">
         <v>1139</v>
       </c>
+      <c r="D157" t="s">
+        <v>1743</v>
+      </c>
       <c r="E157" t="s">
         <v>1140</v>
       </c>
@@ -27605,6 +27626,9 @@
       <c r="C165" t="s">
         <v>418</v>
       </c>
+      <c r="D165" t="s">
+        <v>1745</v>
+      </c>
       <c r="E165" t="s">
         <v>419</v>
       </c>
@@ -27619,6 +27643,9 @@
       <c r="C166" t="s">
         <v>295</v>
       </c>
+      <c r="D166" t="s">
+        <v>1746</v>
+      </c>
       <c r="E166" t="s">
         <v>296</v>
       </c>
@@ -27650,6 +27677,9 @@
       <c r="C168" t="s">
         <v>404</v>
       </c>
+      <c r="D168" t="s">
+        <v>787</v>
+      </c>
       <c r="E168" t="s">
         <v>405</v>
       </c>
@@ -27902,6 +27932,9 @@
       <c r="C183" t="s">
         <v>282</v>
       </c>
+      <c r="D183" t="s">
+        <v>1748</v>
+      </c>
       <c r="E183" t="s">
         <v>283</v>
       </c>
@@ -28035,6 +28068,9 @@
       <c r="C191" t="s">
         <v>1510</v>
       </c>
+      <c r="D191" t="s">
+        <v>567</v>
+      </c>
       <c r="E191" t="s">
         <v>1510</v>
       </c>
@@ -28304,6 +28340,9 @@
       <c r="C207" t="s">
         <v>83</v>
       </c>
+      <c r="D207" t="s">
+        <v>1750</v>
+      </c>
       <c r="E207" t="s">
         <v>84</v>
       </c>
@@ -28335,6 +28374,9 @@
       <c r="C209" t="s">
         <v>286</v>
       </c>
+      <c r="D209" t="s">
+        <v>1747</v>
+      </c>
       <c r="E209" t="s">
         <v>287</v>
       </c>
@@ -28349,6 +28391,9 @@
       <c r="C210" t="s">
         <v>177</v>
       </c>
+      <c r="D210" t="s">
+        <v>1749</v>
+      </c>
       <c r="E210" t="s">
         <v>178</v>
       </c>
@@ -28515,6 +28560,9 @@
       </c>
       <c r="C220" t="s">
         <v>1114</v>
+      </c>
+      <c r="D220" t="s">
+        <v>693</v>
       </c>
       <c r="E220" t="s">
         <v>1115</v>

</xml_diff>